<commit_message>
premiere phase de test - terminée
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
@@ -587,6 +587,28 @@
           <t>pass</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>vmxtbtigbpuvokh@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>vbgpuSZVRQ5</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>